<commit_message>
Update hlr for megneto.softwaretestingboard.com.xlsx
</commit_message>
<xml_diff>
--- a/Extra Work/hlr for megneto.softwaretestingboard.com.xlsx
+++ b/Extra Work/hlr for megneto.softwaretestingboard.com.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NCS\Documents\GitHub\Nirav_Tops\HLR and Testcase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NCS\Documents\GitHub\Nirav_Tops\Extra Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="346">
   <si>
     <t>functionality id</t>
   </si>
@@ -829,18 +829,12 @@
     <t>while clicking on compare button it is working properly and also had open a new page</t>
   </si>
   <si>
-    <t>check remove product close icon</t>
-  </si>
-  <si>
     <t xml:space="preserve">1) https://magento.softwaretestingboard.com
 2) press enter key
 3) click on sign link
 4) click on sign in button
 5) click on training menu
 </t>
-  </si>
-  <si>
-    <t>while clicking on remove product close icon it is working properly and also display a proper message</t>
   </si>
   <si>
     <t>check cancel button</t>
@@ -1552,6 +1546,143 @@
 10) click on add to cart icon
 11) click on proceed to checkout button
 12) click on next button</t>
+  </si>
+  <si>
+    <t>1) https://magento.softwaretestingboard.com
+2) press enter key
+3) click on sign link
+4) click on sign in button
+5) click on women&gt;tops&gt;jackets
+6) click on product link
+7) click on size
+8) click on color
+9) click on add to cart button
+10) click on add to cart icon
+11) click on proceed to checkout button
+12) click on next button
+13) click on place order button</t>
+  </si>
+  <si>
+    <t>1) https://magento.softwaretestingboard.com
+2) press enter key
+3) click on sign link
+4) click on sign in button
+5) click on women&gt;tops&gt;jackets
+6) click on product link
+7) click on size
+8) click on color
+9) click on add to cart button
+10) click on add to cart icon
+11) click on proceed to checkout button
+12) click on next button
+13) click on place order button
+14) click on continue shopping button</t>
+  </si>
+  <si>
+    <t>1) https://magento.softwaretestingboard.com
+2) press enter key
+3) click on sign link
+4) click on sign in button
+5) click on women&gt;tops&gt;jackets
+6) click on product link
+7) click on add to wish list link</t>
+  </si>
+  <si>
+    <t>1) https://magento.softwaretestingboard.com
+2) press enter key
+3) click on sign link
+4) click on sign in button
+5) click on women&gt;tops&gt;jackets
+6) click on product link
+7) click on add to compare link</t>
+  </si>
+  <si>
+    <t>1) https://magento.softwaretestingboard.com
+2) press enter key
+3) click on sign link
+4) click on sign in button
+5) click on women&gt;tops&gt;jackets
+6) click on product link
+7) click on add to wish list link
+8) click on add to compare link
+9) click on comparison list link</t>
+  </si>
+  <si>
+    <t>1) https://magento.softwaretestingboard.com
+2) press enter key
+3) click on sign link
+4) click on sign in button
+5) click on women&gt;tops&gt;jackets
+6) click on product link
+7) click on add to wish list link
+8) click on add to compare link
+9) click on comparison list link
+10) click on compare product link</t>
+  </si>
+  <si>
+    <t>1) https://magento.softwaretestingboard.com
+2) press enter key
+3) click on sign link
+4) click on sign in button
+5) click on women&gt;tops&gt;jackets
+6) click on product link
+7) click on add to wish list link
+8) click on add to compare link
+9) click on compare button</t>
+  </si>
+  <si>
+    <t>check remove this item close icon</t>
+  </si>
+  <si>
+    <t>while clicking on remove this item close icon it is working properly and also display a proper message</t>
+  </si>
+  <si>
+    <t>1) https://magento.softwaretestingboard.com
+2) press enter key
+3) click on sign link
+4) click on sign in button
+5) click on women&gt;tops&gt;jackets
+6) click on product link
+7) click on add to wish list link
+8) click on add to compare link
+9) click on remove this item close icon</t>
+  </si>
+  <si>
+    <t>1) https://magento.softwaretestingboard.com
+2) press enter key
+3) click on sign link
+4) click on sign in button
+5) click on women&gt;tops&gt;jackets
+6) click on product link
+7) click on add to wish list link
+8) click on add to compare link
+9) click on remove this item close icon
+10) click on cancel button</t>
+  </si>
+  <si>
+    <t>1) https://magento.softwaretestingboard.com
+2) press enter key
+3) click on sign link
+4) click on sign in button
+5) click on women&gt;tops&gt;jackets
+6) click on product link
+7) click on add to wish list link
+8) click on add to compare link
+9) click on remove this item close icon
+10) click on ok button</t>
+  </si>
+  <si>
+    <t>1) https://magento.softwaretestingboard.com
+2) press enter key
+3) click on sign link
+4) click on sign in button
+5) click on women&gt;tops&gt;jackets
+6) click on product link
+7) click on add to wish list link
+8) click on add to compare link
+9) click on comparison list link
+10) click on compare product link
+11) click on print this test page link</t>
   </si>
 </sst>
 </file>
@@ -2010,8 +2141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2202,10 +2333,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -2216,7 +2347,7 @@
         <v>73</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -2609,7 +2740,7 @@
         <v>3005</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>94</v>
@@ -2631,10 +2762,10 @@
         <v>3007</v>
       </c>
       <c r="B56" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>302</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -2653,10 +2784,10 @@
         <v>3009</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -2697,10 +2828,10 @@
         <v>3013</v>
       </c>
       <c r="B62" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="C62" s="6" t="s">
         <v>312</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -2994,10 +3125,10 @@
         <v>3040</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>244</v>
+        <v>340</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>246</v>
+        <v>341</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -3005,10 +3136,10 @@
         <v>3041</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -3016,10 +3147,10 @@
         <v>3042</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -3181,8 +3312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C94" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="E104" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I105" sqref="I105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3995,7 +4126,7 @@
         <v>181</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>182</v>
@@ -4024,13 +4155,13 @@
         <v>181</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>182</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H29" s="10" t="s">
         <v>184</v>
@@ -4047,19 +4178,19 @@
         <v>16</v>
       </c>
       <c r="C30" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E30" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>255</v>
-      </c>
       <c r="F30" s="10" t="s">
         <v>182</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H30" s="10" t="s">
         <v>184</v>
@@ -4082,13 +4213,13 @@
         <v>181</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>182</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H31" s="10" t="s">
         <v>184</v>
@@ -4111,7 +4242,7 @@
         <v>181</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>182</v>
@@ -4140,13 +4271,13 @@
         <v>181</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F33" s="10" t="s">
         <v>182</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H33" s="10" t="s">
         <v>184</v>
@@ -4169,13 +4300,13 @@
         <v>181</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>182</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H34" s="10" t="s">
         <v>184</v>
@@ -4198,13 +4329,13 @@
         <v>181</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>182</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H35" s="10" t="s">
         <v>184</v>
@@ -4227,7 +4358,7 @@
         <v>181</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>182</v>
@@ -4256,7 +4387,7 @@
         <v>181</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>182</v>
@@ -4285,7 +4416,7 @@
         <v>181</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F38" s="10" t="s">
         <v>182</v>
@@ -4314,7 +4445,7 @@
         <v>181</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>182</v>
@@ -4343,7 +4474,7 @@
         <v>181</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F40" s="10" t="s">
         <v>182</v>
@@ -4372,7 +4503,7 @@
         <v>181</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F41" s="10" t="s">
         <v>182</v>
@@ -4430,7 +4561,7 @@
         <v>181</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F43" s="10" t="s">
         <v>182</v>
@@ -4459,13 +4590,13 @@
         <v>181</v>
       </c>
       <c r="E44" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="G44" s="4" t="s">
         <v>272</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>274</v>
       </c>
       <c r="H44" s="10" t="s">
         <v>184</v>
@@ -4488,7 +4619,7 @@
         <v>181</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F45" s="10" t="s">
         <v>182</v>
@@ -4517,7 +4648,7 @@
         <v>181</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F46" s="10" t="s">
         <v>182</v>
@@ -4546,7 +4677,7 @@
         <v>181</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>182</v>
@@ -4575,13 +4706,13 @@
         <v>181</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>182</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H48" s="10" t="s">
         <v>184</v>
@@ -4604,7 +4735,7 @@
         <v>181</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>182</v>
@@ -4633,7 +4764,7 @@
         <v>181</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>182</v>
@@ -4662,13 +4793,13 @@
         <v>181</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F51" s="10" t="s">
         <v>182</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H51" s="10" t="s">
         <v>184</v>
@@ -4691,7 +4822,7 @@
         <v>181</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>182</v>
@@ -4720,7 +4851,7 @@
         <v>181</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>182</v>
@@ -4749,7 +4880,7 @@
         <v>181</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>182</v>
@@ -4778,7 +4909,7 @@
         <v>181</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>182</v>
@@ -4807,7 +4938,7 @@
         <v>181</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F56" s="10" t="s">
         <v>182</v>
@@ -4836,7 +4967,7 @@
         <v>181</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F57" s="10" t="s">
         <v>182</v>
@@ -4865,7 +4996,7 @@
         <v>181</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F58" s="10" t="s">
         <v>182</v>
@@ -4894,7 +5025,7 @@
         <v>181</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F59" s="10" t="s">
         <v>182</v>
@@ -4923,13 +5054,13 @@
         <v>181</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F60" s="10" t="s">
         <v>182</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H60" s="10" t="s">
         <v>184</v>
@@ -4952,7 +5083,7 @@
         <v>181</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F61" s="10" t="s">
         <v>182</v>
@@ -4981,7 +5112,7 @@
         <v>181</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F62" s="10" t="s">
         <v>182</v>
@@ -5010,7 +5141,7 @@
         <v>181</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F63" s="10" t="s">
         <v>182</v>
@@ -5039,7 +5170,7 @@
         <v>181</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F64" s="10" t="s">
         <v>182</v>
@@ -5068,7 +5199,7 @@
         <v>181</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F65" s="10" t="s">
         <v>182</v>
@@ -5097,7 +5228,7 @@
         <v>181</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F66" s="10" t="s">
         <v>182</v>
@@ -5120,13 +5251,13 @@
         <v>3005</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D67" s="10" t="s">
         <v>181</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F67" s="10" t="s">
         <v>182</v>
@@ -5155,7 +5286,7 @@
         <v>181</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F68" s="10" t="s">
         <v>182</v>
@@ -5178,19 +5309,19 @@
         <v>3007</v>
       </c>
       <c r="C69" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="G69" s="4" t="s">
         <v>302</v>
-      </c>
-      <c r="D69" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E69" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="F69" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>304</v>
       </c>
       <c r="H69" s="10" t="s">
         <v>184</v>
@@ -5213,7 +5344,7 @@
         <v>181</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F70" s="10" t="s">
         <v>182</v>
@@ -5236,19 +5367,19 @@
         <v>3009</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>181</v>
       </c>
       <c r="E71" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="G71" s="6" t="s">
         <v>306</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="G71" s="6" t="s">
-        <v>308</v>
       </c>
       <c r="H71" s="6" t="s">
         <v>184</v>
@@ -5271,7 +5402,7 @@
         <v>181</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F72" s="10" t="s">
         <v>182</v>
@@ -5300,7 +5431,7 @@
         <v>181</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F73" s="10" t="s">
         <v>182</v>
@@ -5329,7 +5460,7 @@
         <v>181</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F74" s="10" t="s">
         <v>182</v>
@@ -5352,19 +5483,19 @@
         <v>3013</v>
       </c>
       <c r="C75" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E75" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="G75" s="6" t="s">
         <v>312</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="E75" s="12" t="s">
-        <v>313</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="G75" s="6" t="s">
-        <v>314</v>
       </c>
       <c r="H75" s="6" t="s">
         <v>184</v>
@@ -5381,13 +5512,13 @@
         <v>3014</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D76" s="10" t="s">
         <v>181</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F76" s="10" t="s">
         <v>182</v>
@@ -5416,7 +5547,7 @@
         <v>181</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F77" s="10" t="s">
         <v>182</v>
@@ -5445,7 +5576,7 @@
         <v>181</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F78" s="4" t="s">
         <v>182</v>
@@ -5474,7 +5605,7 @@
         <v>181</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F79" s="10" t="s">
         <v>182</v>
@@ -5503,7 +5634,7 @@
         <v>181</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F80" s="10" t="s">
         <v>182</v>
@@ -5532,7 +5663,7 @@
         <v>181</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F81" s="10" t="s">
         <v>182</v>
@@ -5561,7 +5692,7 @@
         <v>181</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F82" s="10" t="s">
         <v>182</v>
@@ -5590,7 +5721,7 @@
         <v>181</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F83" s="10" t="s">
         <v>182</v>
@@ -5619,7 +5750,7 @@
         <v>181</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F84" s="10" t="s">
         <v>182</v>
@@ -5648,7 +5779,7 @@
         <v>181</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F85" s="10" t="s">
         <v>182</v>
@@ -5675,7 +5806,7 @@
         <v>181</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F86" s="10" t="s">
         <v>182</v>
@@ -5704,7 +5835,7 @@
         <v>181</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F87" s="10" t="s">
         <v>182</v>
@@ -5733,7 +5864,7 @@
         <v>181</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F88" s="10" t="s">
         <v>182</v>
@@ -5762,7 +5893,7 @@
         <v>181</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F89" s="10" t="s">
         <v>182</v>
@@ -5791,7 +5922,7 @@
         <v>181</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F90" s="10" t="s">
         <v>182</v>
@@ -5820,7 +5951,7 @@
         <v>181</v>
       </c>
       <c r="E91" s="11" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F91" s="10" t="s">
         <v>182</v>
@@ -5849,7 +5980,7 @@
         <v>181</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F92" s="10" t="s">
         <v>182</v>
@@ -5878,7 +6009,7 @@
         <v>181</v>
       </c>
       <c r="E93" s="11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F93" s="10" t="s">
         <v>182</v>
@@ -5907,7 +6038,7 @@
         <v>181</v>
       </c>
       <c r="E94" s="11" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F94" s="10" t="s">
         <v>182</v>
@@ -5922,7 +6053,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="95" spans="1:9" s="13" customFormat="1" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" s="13" customFormat="1" ht="243.75" x14ac:dyDescent="0.25">
       <c r="A95" s="10">
         <v>94</v>
       </c>
@@ -5936,12 +6067,14 @@
         <v>181</v>
       </c>
       <c r="E95" s="11" t="s">
-        <v>195</v>
+        <v>333</v>
       </c>
       <c r="F95" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="G95" s="10"/>
+      <c r="G95" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="H95" s="10" t="s">
         <v>184</v>
       </c>
@@ -5949,7 +6082,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="96" spans="1:9" s="13" customFormat="1" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" s="13" customFormat="1" ht="262.5" x14ac:dyDescent="0.25">
       <c r="A96" s="10">
         <v>95</v>
       </c>
@@ -5963,12 +6096,14 @@
         <v>181</v>
       </c>
       <c r="E96" s="11" t="s">
-        <v>195</v>
+        <v>334</v>
       </c>
       <c r="F96" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="G96" s="10"/>
+      <c r="G96" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="H96" s="10" t="s">
         <v>184</v>
       </c>
@@ -5976,7 +6111,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="97" spans="1:9" s="13" customFormat="1" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" s="13" customFormat="1" ht="131.25" x14ac:dyDescent="0.25">
       <c r="A97" s="10">
         <v>96</v>
       </c>
@@ -5990,12 +6125,14 @@
         <v>181</v>
       </c>
       <c r="E97" s="11" t="s">
-        <v>195</v>
+        <v>335</v>
       </c>
       <c r="F97" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="G97" s="10"/>
+      <c r="G97" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="H97" s="10" t="s">
         <v>184</v>
       </c>
@@ -6003,7 +6140,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="98" spans="1:9" s="13" customFormat="1" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" s="13" customFormat="1" ht="131.25" x14ac:dyDescent="0.25">
       <c r="A98" s="10">
         <v>97</v>
       </c>
@@ -6017,12 +6154,14 @@
         <v>181</v>
       </c>
       <c r="E98" s="11" t="s">
-        <v>195</v>
+        <v>336</v>
       </c>
       <c r="F98" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="G98" s="10"/>
+      <c r="G98" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="H98" s="10" t="s">
         <v>184</v>
       </c>
@@ -6030,7 +6169,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="99" spans="1:9" s="13" customFormat="1" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" s="13" customFormat="1" ht="168.75" x14ac:dyDescent="0.25">
       <c r="A99" s="10">
         <v>98</v>
       </c>
@@ -6044,12 +6183,14 @@
         <v>181</v>
       </c>
       <c r="E99" s="11" t="s">
-        <v>195</v>
+        <v>337</v>
       </c>
       <c r="F99" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="G99" s="10"/>
+      <c r="G99" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="H99" s="10" t="s">
         <v>184</v>
       </c>
@@ -6057,7 +6198,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="100" spans="1:9" s="13" customFormat="1" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" s="13" customFormat="1" ht="187.5" x14ac:dyDescent="0.25">
       <c r="A100" s="10">
         <v>99</v>
       </c>
@@ -6071,12 +6212,14 @@
         <v>181</v>
       </c>
       <c r="E100" s="11" t="s">
-        <v>195</v>
+        <v>338</v>
       </c>
       <c r="F100" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="G100" s="10"/>
+      <c r="G100" s="4" t="s">
+        <v>170</v>
+      </c>
       <c r="H100" s="10" t="s">
         <v>184</v>
       </c>
@@ -6084,26 +6227,28 @@
         <v>185</v>
       </c>
     </row>
-    <row r="101" spans="1:9" s="13" customFormat="1" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" s="13" customFormat="1" ht="168.75" x14ac:dyDescent="0.25">
       <c r="A101" s="10">
         <v>100</v>
       </c>
       <c r="B101" s="10">
         <v>3039</v>
       </c>
-      <c r="C101" s="10" t="s">
-        <v>100</v>
+      <c r="C101" s="4" t="s">
+        <v>242</v>
       </c>
       <c r="D101" s="10" t="s">
         <v>181</v>
       </c>
       <c r="E101" s="11" t="s">
-        <v>195</v>
+        <v>339</v>
       </c>
       <c r="F101" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="G101" s="10"/>
+      <c r="G101" s="4" t="s">
+        <v>243</v>
+      </c>
       <c r="H101" s="10" t="s">
         <v>184</v>
       </c>
@@ -6111,25 +6256,28 @@
         <v>185</v>
       </c>
     </row>
-    <row r="102" spans="1:9" s="13" customFormat="1" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" s="13" customFormat="1" ht="168.75" x14ac:dyDescent="0.25">
       <c r="A102" s="10">
         <v>101</v>
       </c>
       <c r="B102" s="10">
         <v>3040</v>
       </c>
-      <c r="C102" s="10" t="s">
-        <v>102</v>
+      <c r="C102" s="4" t="s">
+        <v>340</v>
       </c>
       <c r="D102" s="10" t="s">
         <v>181</v>
       </c>
       <c r="E102" s="11" t="s">
-        <v>195</v>
+        <v>342</v>
       </c>
       <c r="F102" s="10" t="s">
         <v>182</v>
       </c>
+      <c r="G102" s="4" t="s">
+        <v>341</v>
+      </c>
       <c r="H102" s="10" t="s">
         <v>184</v>
       </c>
@@ -6137,25 +6285,28 @@
         <v>185</v>
       </c>
     </row>
-    <row r="103" spans="1:9" s="13" customFormat="1" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" s="13" customFormat="1" ht="187.5" x14ac:dyDescent="0.25">
       <c r="A103" s="10">
         <v>102</v>
       </c>
       <c r="B103" s="10">
         <v>3041</v>
       </c>
-      <c r="C103" s="10" t="s">
-        <v>104</v>
+      <c r="C103" s="4" t="s">
+        <v>245</v>
       </c>
       <c r="D103" s="10" t="s">
         <v>181</v>
       </c>
       <c r="E103" s="11" t="s">
-        <v>195</v>
+        <v>343</v>
       </c>
       <c r="F103" s="10" t="s">
         <v>182</v>
       </c>
+      <c r="G103" s="4" t="s">
+        <v>246</v>
+      </c>
       <c r="H103" s="10" t="s">
         <v>184</v>
       </c>
@@ -6163,25 +6314,28 @@
         <v>185</v>
       </c>
     </row>
-    <row r="104" spans="1:9" s="13" customFormat="1" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" s="13" customFormat="1" ht="187.5" x14ac:dyDescent="0.25">
       <c r="A104" s="10">
         <v>103</v>
       </c>
       <c r="B104" s="10">
         <v>3042</v>
       </c>
-      <c r="C104" s="10" t="s">
-        <v>106</v>
+      <c r="C104" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="D104" s="10" t="s">
         <v>181</v>
       </c>
       <c r="E104" s="11" t="s">
-        <v>195</v>
+        <v>344</v>
       </c>
       <c r="F104" s="10" t="s">
         <v>182</v>
       </c>
+      <c r="G104" s="4" t="s">
+        <v>248</v>
+      </c>
       <c r="H104" s="10" t="s">
         <v>184</v>
       </c>
@@ -6189,24 +6343,27 @@
         <v>185</v>
       </c>
     </row>
-    <row r="105" spans="1:9" s="13" customFormat="1" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" s="13" customFormat="1" ht="206.25" x14ac:dyDescent="0.25">
       <c r="A105" s="10">
         <v>104</v>
       </c>
       <c r="B105" s="10">
         <v>3043</v>
       </c>
-      <c r="C105" s="10" t="s">
-        <v>108</v>
+      <c r="C105" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="D105" s="10" t="s">
         <v>181</v>
       </c>
       <c r="E105" s="11" t="s">
-        <v>195</v>
+        <v>345</v>
       </c>
       <c r="F105" s="10" t="s">
         <v>182</v>
+      </c>
+      <c r="G105" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="H105" s="10" t="s">
         <v>184</v>
@@ -6222,8 +6379,8 @@
       <c r="B106" s="10">
         <v>3044</v>
       </c>
-      <c r="C106" s="10" t="s">
-        <v>110</v>
+      <c r="C106" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="D106" s="10" t="s">
         <v>181</v>
@@ -6248,8 +6405,8 @@
       <c r="B107" s="10">
         <v>3045</v>
       </c>
-      <c r="C107" s="10" t="s">
-        <v>112</v>
+      <c r="C107" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="D107" s="10" t="s">
         <v>181</v>
@@ -6274,8 +6431,8 @@
       <c r="B108" s="10">
         <v>3046</v>
       </c>
-      <c r="C108" s="10" t="s">
-        <v>114</v>
+      <c r="C108" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="D108" s="10" t="s">
         <v>181</v>
@@ -6300,8 +6457,8 @@
       <c r="B109" s="10">
         <v>3047</v>
       </c>
-      <c r="C109" s="10" t="s">
-        <v>116</v>
+      <c r="C109" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="D109" s="10" t="s">
         <v>181</v>
@@ -6323,6 +6480,9 @@
       <c r="A110" s="10">
         <v>109</v>
       </c>
+      <c r="C110" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="D110" s="10" t="s">
         <v>181</v>
       </c>
@@ -6343,6 +6503,9 @@
       <c r="A111" s="10">
         <v>110</v>
       </c>
+      <c r="C111" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="D111" s="10" t="s">
         <v>181</v>
       </c>
@@ -6363,6 +6526,9 @@
       <c r="A112" s="10">
         <v>111</v>
       </c>
+      <c r="C112" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="D112" s="10" t="s">
         <v>181</v>
       </c>
@@ -6382,6 +6548,9 @@
     <row r="113" spans="1:9" s="13" customFormat="1" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A113" s="10">
         <v>112</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="D113" s="10" t="s">
         <v>181</v>

</xml_diff>